<commit_message>
Added rendered HTML code
</commit_message>
<xml_diff>
--- a/data/examples/webdev/datafile.xlsx
+++ b/data/examples/webdev/datafile.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7DC889-641A-604E-9034-6ED86752B5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F85B28-5783-FD4A-908D-1C9CCE019B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="webdev-home" sheetId="1" r:id="rId1"/>
-    <sheet name="webdev-mishipay" sheetId="2" r:id="rId2"/>
+    <sheet name="webdev-home-mishipay" sheetId="1" r:id="rId1"/>
+    <sheet name="webdev-mishipay-hero" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -94,6 +94,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">

</xml_diff>